<commit_message>
Changed UDC name from ExcelUdc to iPortal
</commit_message>
<xml_diff>
--- a/udc/local_users_db.xlsx
+++ b/udc/local_users_db.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tom\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -157,7 +157,7 @@
     <t>udc</t>
   </si>
   <si>
-    <t>EXCELUDC</t>
+    <t>iPortal</t>
   </si>
 </sst>
 </file>
@@ -1107,8 +1107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58:C66"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58:C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>